<commit_message>
Trabajos, mejoras de optimización
</commit_message>
<xml_diff>
--- a/public/database/Usuarios.xlsx
+++ b/public/database/Usuarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio Aguilera\Desktop\Trabajo (SPA)\ProyectoReact\public\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2DF8D2-28CA-4549-8E42-A4EA026AA8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D847FC1E-A8CB-41CE-8458-F001B1DAC2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D68F4056-0D45-4BC6-8B04-16C26C5398A7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>usuario</t>
   </si>
@@ -61,6 +61,21 @@
   </si>
   <si>
     <t>$2b$10$7JyEmv1DMcHUfsKb/JagS.j4Vrzh/hvOTBN7JeVZF2Ry2R4G8v4IG</t>
+  </si>
+  <si>
+    <t>iaguilera</t>
+  </si>
+  <si>
+    <t>Ignacio Aguilera</t>
+  </si>
+  <si>
+    <t>$2b$10$NKSgcAXRuxSqKkECocB2/egUEGcVN02XkKrVpbmFo3js.gGmrrtQu</t>
+  </si>
+  <si>
+    <t>alias</t>
+  </si>
+  <si>
+    <t>Maicita</t>
   </si>
 </sst>
 </file>
@@ -426,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9B6F27-5EFA-4ABC-AF87-8DE32F38EB28}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,7 +453,7 @@
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,8 +463,11 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -459,8 +477,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -469,6 +490,23 @@
       </c>
       <c r="C3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>